<commit_message>
ny farve på figur
i mean why the fuck er den ene farve blå og den anden farve mørke blå det giver ingen mening
</commit_message>
<xml_diff>
--- a/MATLAB/Målinger.xlsx
+++ b/MATLAB/Målinger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilt\Documents\Robotics\P3\GitHub\2020-11-18\P3\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0DE076D-82CE-4EDD-B703-8FB35DCDA935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C89F6763-AE59-48CD-A92C-8CCDF132265D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{78552C7D-3AD2-4F19-ADA0-D8702E4DDCDF}"/>
   </bookViews>
@@ -15138,12 +15138,13 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="3175">
                 <a:solidFill>
-                  <a:schemeClr val="accent5"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -42435,11 +42436,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="B2:O2"/>
     <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AE2:AO2"/>
     <mergeCell ref="Q2:AA2"/>
@@ -42449,6 +42445,11 @@
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="B2:O2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="H5:I5"/>
@@ -42503,21 +42504,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BA49DA1804610541B0C7F37312C70C1C" ma:contentTypeVersion="10" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="3c673c20184515bb2fc3611307108fd1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3946d706-8ec9-4b4d-aeb9-fc69995c0d30" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c52a18275b7a723dee42e83b498ddce8" ns2:_="">
     <xsd:import namespace="3946d706-8ec9-4b4d-aeb9-fc69995c0d30"/>
@@ -42701,8 +42687,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533245B6-113D-47E5-9B6C-1D49A6452BAC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25503C7E-8637-4AEF-8E65-D52CF9C39D34}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42710,5 +42711,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25503C7E-8637-4AEF-8E65-D52CF9C39D34}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533245B6-113D-47E5-9B6C-1D49A6452BAC}"/>
 </file>
</xml_diff>